<commit_message>
Fuegt zusaetzliche Operations hinzu
- GET /api/alarms mit AlarmID
- DELETE /api/devices mit DeviceID
- DELETE /api/actiongroupmembers mit DeviceID (loescht aus allen Gruppen)
- DELETE /api/actiongroupmembers mit GroupID (loescht ganze Gruppe)
</commit_message>
<xml_diff>
--- a/doku/WI27_WebService.Definition.xlsx
+++ b/doku/WI27_WebService.Definition.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17426"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Markus\Documents\FFHS\git\ESHH\doku\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Markus\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="155">
   <si>
     <t>GetDevice</t>
   </si>
@@ -477,6 +477,21 @@
   </si>
   <si>
     <t>Löscht das ActionGroupMember mit der DeviceID aus der ActionGroup mit GroupID</t>
+  </si>
+  <si>
+    <t>Löscht das Device aus allen ActionGroups</t>
+  </si>
+  <si>
+    <t>Löscht die ganze ActionGroup mit der GroupID</t>
+  </si>
+  <si>
+    <t>Löscht das Device mit der DeviceID</t>
+  </si>
+  <si>
+    <t>AlarmID</t>
+  </si>
+  <si>
+    <t>Gibt den Alarm mit der AlarmID zurück</t>
   </si>
 </sst>
 </file>
@@ -555,42 +570,6 @@
   </cellStyles>
   <dxfs count="9">
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -615,6 +594,9 @@
       </font>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -623,6 +605,39 @@
         <family val="2"/>
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -669,17 +684,17 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:I18" totalsRowShown="0">
-  <autoFilter ref="A1:I18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:I22" totalsRowShown="0">
+  <autoFilter ref="A1:I22">
     <filterColumn colId="0">
       <filters>
-        <filter val="POST"/>
+        <filter val="GET"/>
       </filters>
     </filterColumn>
   </autoFilter>
   <tableColumns count="9">
-    <tableColumn id="5" name="Operation" dataDxfId="0"/>
-    <tableColumn id="1" name="URL" dataDxfId="1"/>
+    <tableColumn id="5" name="Operation" dataDxfId="7"/>
+    <tableColumn id="1" name="URL" dataDxfId="6"/>
     <tableColumn id="2" name="Parameter 1"/>
     <tableColumn id="3" name="Parameter 2"/>
     <tableColumn id="6" name="Parameter 3"/>
@@ -711,12 +726,12 @@
     <tableColumn id="1" name="URL"/>
     <tableColumn id="9" name="Operation"/>
     <tableColumn id="2" name="Parameter"/>
-    <tableColumn id="3" name="Opt." dataDxfId="7"/>
-    <tableColumn id="4" name="Beispiel" dataDxfId="6"/>
+    <tableColumn id="3" name="Opt." dataDxfId="5"/>
+    <tableColumn id="4" name="Beispiel" dataDxfId="4"/>
     <tableColumn id="5" name="DB-Feld"/>
     <tableColumn id="6" name="Typ"/>
     <tableColumn id="7" name="Unique"/>
-    <tableColumn id="11" name="Example" dataDxfId="2">
+    <tableColumn id="11" name="Example" dataDxfId="3">
       <calculatedColumnFormula>_xlfn.CONCAT(Table8[[#This Row],[URL]],"?",Table8[[#This Row],[Parameter]],"=",Table8[[#This Row],[Beispiel]])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="8" name="Kommentar"/>
@@ -726,13 +741,13 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Table1313" displayName="Table1313" ref="A1:G51" totalsRowShown="0" headerRowDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Table1313" displayName="Table1313" ref="A1:G51" totalsRowShown="0" headerRowDxfId="2">
   <autoFilter ref="A1:G51"/>
   <tableColumns count="7">
     <tableColumn id="1" name="Operation"/>
     <tableColumn id="5" name="Feld"/>
-    <tableColumn id="3" name="Anzahl" dataDxfId="4"/>
-    <tableColumn id="4" name="Beispiel" dataDxfId="3"/>
+    <tableColumn id="3" name="Anzahl" dataDxfId="1"/>
+    <tableColumn id="4" name="Beispiel" dataDxfId="0"/>
     <tableColumn id="6" name="DB-Feld"/>
     <tableColumn id="7" name="Typ"/>
     <tableColumn id="10" name="Kommentar"/>
@@ -1087,11 +1102,11 @@
         <v>42</v>
       </c>
       <c r="I2" s="4" t="str">
-        <f>_xlfn.CONCAT(A2,"Request")</f>
+        <f t="shared" ref="I2:I17" si="0">_xlfn.CONCAT(A2,"Request")</f>
         <v>GetDeviceRequest</v>
       </c>
       <c r="J2" s="4" t="str">
-        <f>_xlfn.CONCAT(A2,"Response")</f>
+        <f t="shared" ref="J2:J17" si="1">_xlfn.CONCAT(A2,"Response")</f>
         <v>GetDeviceResponse</v>
       </c>
     </row>
@@ -1109,11 +1124,11 @@
         <v>43</v>
       </c>
       <c r="I3" s="4" t="str">
-        <f>_xlfn.CONCAT(A3,"Request")</f>
+        <f t="shared" si="0"/>
         <v>AddDeviceRequest</v>
       </c>
       <c r="J3" s="4" t="str">
-        <f>_xlfn.CONCAT(A3,"Response")</f>
+        <f t="shared" si="1"/>
         <v>AddDeviceResponse</v>
       </c>
     </row>
@@ -1131,11 +1146,11 @@
         <v>44</v>
       </c>
       <c r="I4" s="4" t="str">
-        <f>_xlfn.CONCAT(A4,"Request")</f>
+        <f t="shared" si="0"/>
         <v>RemoveDeviceRequest</v>
       </c>
       <c r="J4" s="4" t="str">
-        <f>_xlfn.CONCAT(A4,"Response")</f>
+        <f t="shared" si="1"/>
         <v>RemoveDeviceResponse</v>
       </c>
     </row>
@@ -1153,11 +1168,11 @@
         <v>40</v>
       </c>
       <c r="I5" t="str">
-        <f>_xlfn.CONCAT(A5,"Request")</f>
+        <f t="shared" si="0"/>
         <v>GetAlarmRequest</v>
       </c>
       <c r="J5" t="str">
-        <f>_xlfn.CONCAT(A5,"Response")</f>
+        <f t="shared" si="1"/>
         <v>GetAlarmResponse</v>
       </c>
     </row>
@@ -1175,11 +1190,11 @@
         <v>39</v>
       </c>
       <c r="I6" t="str">
-        <f>_xlfn.CONCAT(A6,"Request")</f>
+        <f t="shared" si="0"/>
         <v>AddAlarmRequest</v>
       </c>
       <c r="J6" t="str">
-        <f>_xlfn.CONCAT(A6,"Response")</f>
+        <f t="shared" si="1"/>
         <v>AddAlarmResponse</v>
       </c>
     </row>
@@ -1197,11 +1212,11 @@
         <v>41</v>
       </c>
       <c r="I7" t="str">
-        <f>_xlfn.CONCAT(A7,"Request")</f>
+        <f t="shared" si="0"/>
         <v>RemoveAlarmRequest</v>
       </c>
       <c r="J7" t="str">
-        <f>_xlfn.CONCAT(A7,"Response")</f>
+        <f t="shared" si="1"/>
         <v>RemoveAlarmResponse</v>
       </c>
     </row>
@@ -1219,11 +1234,11 @@
         <v>40</v>
       </c>
       <c r="I8" t="str">
-        <f>_xlfn.CONCAT(A8,"Request")</f>
+        <f t="shared" si="0"/>
         <v>GetDeviceActionRequest</v>
       </c>
       <c r="J8" t="str">
-        <f>_xlfn.CONCAT(A8,"Response")</f>
+        <f t="shared" si="1"/>
         <v>GetDeviceActionResponse</v>
       </c>
     </row>
@@ -1241,11 +1256,11 @@
         <v>39</v>
       </c>
       <c r="I9" t="str">
-        <f>_xlfn.CONCAT(A9,"Request")</f>
+        <f t="shared" si="0"/>
         <v>AddDeviceActionRequest</v>
       </c>
       <c r="J9" t="str">
-        <f>_xlfn.CONCAT(A9,"Response")</f>
+        <f t="shared" si="1"/>
         <v>AddDeviceActionResponse</v>
       </c>
     </row>
@@ -1263,11 +1278,11 @@
         <v>41</v>
       </c>
       <c r="I10" t="str">
-        <f>_xlfn.CONCAT(A10,"Request")</f>
+        <f t="shared" si="0"/>
         <v>RemoveDeviceActionRequest</v>
       </c>
       <c r="J10" t="str">
-        <f>_xlfn.CONCAT(A10,"Response")</f>
+        <f t="shared" si="1"/>
         <v>RemoveDeviceActionResponse</v>
       </c>
     </row>
@@ -1285,11 +1300,11 @@
         <v>40</v>
       </c>
       <c r="I11" t="str">
-        <f>_xlfn.CONCAT(A11,"Request")</f>
+        <f t="shared" si="0"/>
         <v>GetActionGroupMemberRequest</v>
       </c>
       <c r="J11" t="str">
-        <f>_xlfn.CONCAT(A11,"Response")</f>
+        <f t="shared" si="1"/>
         <v>GetActionGroupMemberResponse</v>
       </c>
     </row>
@@ -1307,11 +1322,11 @@
         <v>39</v>
       </c>
       <c r="I12" t="str">
-        <f>_xlfn.CONCAT(A12,"Request")</f>
+        <f t="shared" si="0"/>
         <v>AddActionGroupMemberRequest</v>
       </c>
       <c r="J12" t="str">
-        <f>_xlfn.CONCAT(A12,"Response")</f>
+        <f t="shared" si="1"/>
         <v>AddActionGroupMemberResponse</v>
       </c>
     </row>
@@ -1329,11 +1344,11 @@
         <v>41</v>
       </c>
       <c r="I13" t="str">
-        <f>_xlfn.CONCAT(A13,"Request")</f>
+        <f t="shared" si="0"/>
         <v>RemoveActionGroupMemberRequest</v>
       </c>
       <c r="J13" t="str">
-        <f>_xlfn.CONCAT(A13,"Response")</f>
+        <f t="shared" si="1"/>
         <v>RemoveActionGroupMemberResponse</v>
       </c>
     </row>
@@ -1351,11 +1366,11 @@
         <v>47</v>
       </c>
       <c r="I14" t="str">
-        <f>_xlfn.CONCAT(A14,"Request")</f>
+        <f t="shared" si="0"/>
         <v>ActivateActionGroupRequest</v>
       </c>
       <c r="J14" t="str">
-        <f>_xlfn.CONCAT(A14,"Response")</f>
+        <f t="shared" si="1"/>
         <v>ActivateActionGroupResponse</v>
       </c>
     </row>
@@ -1373,11 +1388,11 @@
         <v>48</v>
       </c>
       <c r="I15" t="str">
-        <f>_xlfn.CONCAT(A15,"Request")</f>
+        <f t="shared" si="0"/>
         <v>DisableActionGroupRequest</v>
       </c>
       <c r="J15" t="str">
-        <f>_xlfn.CONCAT(A15,"Response")</f>
+        <f t="shared" si="1"/>
         <v>DisableActionGroupResponse</v>
       </c>
     </row>
@@ -1395,11 +1410,11 @@
         <v>51</v>
       </c>
       <c r="I16" t="str">
-        <f>_xlfn.CONCAT(A16,"Request")</f>
+        <f t="shared" si="0"/>
         <v>ActivateNightLightRequest</v>
       </c>
       <c r="J16" t="str">
-        <f>_xlfn.CONCAT(A16,"Response")</f>
+        <f t="shared" si="1"/>
         <v>ActivateNightLightResponse</v>
       </c>
     </row>
@@ -1417,11 +1432,11 @@
         <v>52</v>
       </c>
       <c r="I17" t="str">
-        <f>_xlfn.CONCAT(A17,"Request")</f>
+        <f t="shared" si="0"/>
         <v>DisableNightLightRequest</v>
       </c>
       <c r="J17" t="str">
-        <f>_xlfn.CONCAT(A17,"Response")</f>
+        <f t="shared" si="1"/>
         <v>DisableNightLightResponse</v>
       </c>
     </row>
@@ -1435,10 +1450,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1479,7 +1494,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>109</v>
       </c>
@@ -1490,7 +1505,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>109</v>
       </c>
@@ -1504,7 +1519,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>109</v>
       </c>
@@ -1515,88 +1530,85 @@
         <v>127</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>109</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" t="s">
-        <v>10</v>
+        <v>153</v>
       </c>
       <c r="I5" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>109</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C6" t="s">
-        <v>80</v>
+        <v>12</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
       </c>
       <c r="I6" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>109</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C7" t="s">
         <v>80</v>
       </c>
       <c r="I7" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>109</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C8" t="s">
         <v>80</v>
       </c>
       <c r="I8" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>109</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" t="s">
-        <v>10</v>
+        <v>80</v>
       </c>
       <c r="I9" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>109</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C10" t="s">
         <v>12</v>
@@ -1605,116 +1617,119 @@
         <v>10</v>
       </c>
       <c r="I10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="C11" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="D11" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="I11" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>110</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C12" t="s">
-        <v>58</v>
+        <v>3</v>
       </c>
       <c r="D12" t="s">
-        <v>61</v>
+        <v>12</v>
       </c>
       <c r="E12" t="s">
-        <v>64</v>
-      </c>
-      <c r="F12" t="s">
-        <v>68</v>
-      </c>
-      <c r="G12" t="s">
-        <v>69</v>
+        <v>14</v>
       </c>
       <c r="I12" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>110</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C13" t="s">
-        <v>12</v>
+        <v>58</v>
       </c>
       <c r="D13" t="s">
-        <v>141</v>
+        <v>61</v>
       </c>
       <c r="E13" t="s">
-        <v>142</v>
+        <v>64</v>
       </c>
       <c r="F13" t="s">
-        <v>143</v>
+        <v>68</v>
       </c>
       <c r="G13" t="s">
-        <v>107</v>
+        <v>69</v>
       </c>
       <c r="I13" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>110</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C14" t="s">
-        <v>80</v>
+        <v>12</v>
       </c>
       <c r="D14" t="s">
-        <v>83</v>
+        <v>141</v>
       </c>
       <c r="E14" t="s">
-        <v>81</v>
+        <v>142</v>
       </c>
       <c r="F14" t="s">
-        <v>61</v>
+        <v>143</v>
+      </c>
+      <c r="G14" t="s">
+        <v>107</v>
       </c>
       <c r="I14" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="C15" t="s">
-        <v>12</v>
+        <v>80</v>
+      </c>
+      <c r="D15" t="s">
+        <v>83</v>
+      </c>
+      <c r="E15" t="s">
+        <v>81</v>
+      </c>
+      <c r="F15" t="s">
+        <v>61</v>
       </c>
       <c r="I15" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -1722,13 +1737,13 @@
         <v>113</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C16" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="I16" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -1736,16 +1751,13 @@
         <v>113</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C17" t="s">
-        <v>12</v>
-      </c>
-      <c r="D17" t="s">
-        <v>10</v>
+        <v>83</v>
       </c>
       <c r="I17" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -1753,16 +1765,75 @@
         <v>113</v>
       </c>
       <c r="B18" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="C18" t="s">
+        <v>10</v>
+      </c>
+      <c r="I18" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="C19" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" t="s">
+        <v>10</v>
+      </c>
+      <c r="I19" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="B20" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C20" t="s">
         <v>80</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D20" t="s">
         <v>83</v>
       </c>
-      <c r="I18" t="s">
+      <c r="I20" t="s">
         <v>149</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="C21" t="s">
+        <v>83</v>
+      </c>
+      <c r="I21" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="C22" t="s">
+        <v>80</v>
+      </c>
+      <c r="I22" t="s">
+        <v>151</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Beschreibt die WebService Funktionen für Nightlight und ActionGroup
</commit_message>
<xml_diff>
--- a/doku/WI27_WebService.Definition.xlsx
+++ b/doku/WI27_WebService.Definition.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Markus\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Markus\Documents\FFHS\git\ESHH\doku\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="159">
   <si>
     <t>GetDevice</t>
   </si>
@@ -431,12 +431,6 @@
     <t>Deaktiviert die ActionGroup mit der angegebenen GroupID</t>
   </si>
   <si>
-    <t>Aktiviert das angegebene Gerät mit der angegebenen DeviceAction</t>
-  </si>
-  <si>
-    <t>Deaktiviert die angegebene DeviceAction &lt;ID&gt; auf dem angegebenen Device &lt;StringID&gt;</t>
-  </si>
-  <si>
     <t>Fügt ein neues Gerät ein</t>
   </si>
   <si>
@@ -492,6 +486,24 @@
   </si>
   <si>
     <t>Gibt den Alarm mit der AlarmID zurück</t>
+  </si>
+  <si>
+    <t>Aktiviert das angegebene Gerät mit der angegebenen DeviceAction, gibt die aktivierte ActionGroup zurück</t>
+  </si>
+  <si>
+    <t>Deaktiviert die angegebene DeviceAction &lt;ID&gt; auf dem angegebenen Device &lt;StringID&gt;, gibt die deaktivierte ActionGroup zurück</t>
+  </si>
+  <si>
+    <t>/api/nightlight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gibt alle aktivierten Nightlights als ActionGroups zurück </t>
+  </si>
+  <si>
+    <t>/api/actiongroup</t>
+  </si>
+  <si>
+    <t>Gibt alle manuell aktivierten ActionGroups zurück</t>
   </si>
 </sst>
 </file>
@@ -684,8 +696,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:I22" totalsRowShown="0">
-  <autoFilter ref="A1:I22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:I24" totalsRowShown="0">
+  <autoFilter ref="A1:I24">
     <filterColumn colId="0">
       <filters>
         <filter val="GET"/>
@@ -1450,10 +1462,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1482,13 +1494,13 @@
         <v>129</v>
       </c>
       <c r="F1" t="s">
+        <v>136</v>
+      </c>
+      <c r="G1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H1" t="s">
         <v>138</v>
-      </c>
-      <c r="G1" t="s">
-        <v>137</v>
-      </c>
-      <c r="H1" t="s">
-        <v>140</v>
       </c>
       <c r="I1" t="s">
         <v>125</v>
@@ -1538,10 +1550,10 @@
         <v>112</v>
       </c>
       <c r="C5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I5" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -1613,11 +1625,8 @@
       <c r="C10" t="s">
         <v>12</v>
       </c>
-      <c r="D10" t="s">
-        <v>10</v>
-      </c>
       <c r="I10" t="s">
-        <v>134</v>
+        <v>153</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -1630,11 +1639,8 @@
       <c r="C11" t="s">
         <v>12</v>
       </c>
-      <c r="D11" t="s">
-        <v>10</v>
-      </c>
       <c r="I11" t="s">
-        <v>135</v>
+        <v>154</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -1654,7 +1660,7 @@
         <v>14</v>
       </c>
       <c r="I12" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -1680,7 +1686,7 @@
         <v>69</v>
       </c>
       <c r="I13" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -1694,19 +1700,19 @@
         <v>12</v>
       </c>
       <c r="D14" t="s">
+        <v>139</v>
+      </c>
+      <c r="E14" t="s">
+        <v>140</v>
+      </c>
+      <c r="F14" t="s">
         <v>141</v>
-      </c>
-      <c r="E14" t="s">
-        <v>142</v>
-      </c>
-      <c r="F14" t="s">
-        <v>143</v>
       </c>
       <c r="G14" t="s">
         <v>107</v>
       </c>
       <c r="I14" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -1729,7 +1735,7 @@
         <v>61</v>
       </c>
       <c r="I15" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -1743,7 +1749,7 @@
         <v>12</v>
       </c>
       <c r="I16" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -1757,7 +1763,7 @@
         <v>83</v>
       </c>
       <c r="I17" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -1771,7 +1777,7 @@
         <v>10</v>
       </c>
       <c r="I18" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -1788,7 +1794,7 @@
         <v>10</v>
       </c>
       <c r="I19" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -1805,7 +1811,7 @@
         <v>83</v>
       </c>
       <c r="I20" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -1819,7 +1825,7 @@
         <v>83</v>
       </c>
       <c r="I21" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
@@ -1833,7 +1839,29 @@
         <v>80</v>
       </c>
       <c r="I22" t="s">
-        <v>151</v>
+        <v>149</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="I23" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="I24" t="s">
+        <v>158</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fuehrt Dokumentation mit Associate / Disassociate Funktionen nach
</commit_message>
<xml_diff>
--- a/doku/WI27_WebService.Definition.xlsx
+++ b/doku/WI27_WebService.Definition.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="163">
   <si>
     <t>GetDevice</t>
   </si>
@@ -504,6 +504,18 @@
   </si>
   <si>
     <t>Gibt alle manuell aktivierten ActionGroups zurück</t>
+  </si>
+  <si>
+    <t>/api/nightlight/associate</t>
+  </si>
+  <si>
+    <t>Assoziiert die StringID mit der GroupID als Nachtlicht</t>
+  </si>
+  <si>
+    <t>/api/nightlight/disassociate</t>
+  </si>
+  <si>
+    <t>Entfernt die StringID mit der GroupID als Nachtlicht</t>
   </si>
 </sst>
 </file>
@@ -582,6 +594,39 @@
   </cellStyles>
   <dxfs count="9">
     <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -617,39 +662,6 @@
         <family val="2"/>
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -696,8 +708,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:I24" totalsRowShown="0">
-  <autoFilter ref="A1:I24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:I26" totalsRowShown="0">
+  <autoFilter ref="A1:I26">
     <filterColumn colId="0">
       <filters>
         <filter val="GET"/>
@@ -705,8 +717,8 @@
     </filterColumn>
   </autoFilter>
   <tableColumns count="9">
-    <tableColumn id="5" name="Operation" dataDxfId="7"/>
-    <tableColumn id="1" name="URL" dataDxfId="6"/>
+    <tableColumn id="5" name="Operation" dataDxfId="1"/>
+    <tableColumn id="1" name="URL" dataDxfId="0"/>
     <tableColumn id="2" name="Parameter 1"/>
     <tableColumn id="3" name="Parameter 2"/>
     <tableColumn id="6" name="Parameter 3"/>
@@ -738,12 +750,12 @@
     <tableColumn id="1" name="URL"/>
     <tableColumn id="9" name="Operation"/>
     <tableColumn id="2" name="Parameter"/>
-    <tableColumn id="3" name="Opt." dataDxfId="5"/>
-    <tableColumn id="4" name="Beispiel" dataDxfId="4"/>
+    <tableColumn id="3" name="Opt." dataDxfId="7"/>
+    <tableColumn id="4" name="Beispiel" dataDxfId="6"/>
     <tableColumn id="5" name="DB-Feld"/>
     <tableColumn id="6" name="Typ"/>
     <tableColumn id="7" name="Unique"/>
-    <tableColumn id="11" name="Example" dataDxfId="3">
+    <tableColumn id="11" name="Example" dataDxfId="5">
       <calculatedColumnFormula>_xlfn.CONCAT(Table8[[#This Row],[URL]],"?",Table8[[#This Row],[Parameter]],"=",Table8[[#This Row],[Beispiel]])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="8" name="Kommentar"/>
@@ -753,13 +765,13 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Table1313" displayName="Table1313" ref="A1:G51" totalsRowShown="0" headerRowDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Table1313" displayName="Table1313" ref="A1:G51" totalsRowShown="0" headerRowDxfId="4">
   <autoFilter ref="A1:G51"/>
   <tableColumns count="7">
     <tableColumn id="1" name="Operation"/>
     <tableColumn id="5" name="Feld"/>
-    <tableColumn id="3" name="Anzahl" dataDxfId="1"/>
-    <tableColumn id="4" name="Beispiel" dataDxfId="0"/>
+    <tableColumn id="3" name="Anzahl" dataDxfId="3"/>
+    <tableColumn id="4" name="Beispiel" dataDxfId="2"/>
     <tableColumn id="6" name="DB-Feld"/>
     <tableColumn id="7" name="Typ"/>
     <tableColumn id="10" name="Kommentar"/>
@@ -1462,10 +1474,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1847,10 +1859,16 @@
         <v>109</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>155</v>
+        <v>159</v>
+      </c>
+      <c r="C23" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" t="s">
+        <v>80</v>
       </c>
       <c r="I23" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -1858,9 +1876,37 @@
         <v>109</v>
       </c>
       <c r="B24" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="C24" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24" t="s">
+        <v>80</v>
+      </c>
+      <c r="I24" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="I25" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B26" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="I24" t="s">
+      <c r="I26" t="s">
         <v>158</v>
       </c>
     </row>

</xml_diff>